<commit_message>
Additional data in excel sheet
</commit_message>
<xml_diff>
--- a/Files/Parameter Optimization_Planning Sheet.xlsx
+++ b/Files/Parameter Optimization_Planning Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2d90ee17b1e0b34/Git Hub/API/AUTOMATION/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivikram\OneDrive\Git Hub\API\AUTOMATION\parameter_optimization\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{7BD3B360-EE1E-48D4-B04B-4EECFC82A97E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B7E9EA37-E9E8-410E-9561-598D64BFD6EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D796473-49F0-42ED-A728-9DAC3B26F8FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -318,24 +318,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -345,6 +333,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,14 +647,14 @@
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16">
+      <c r="B1" s="13">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="F1" s="10" t="s">
+      <c r="D1" s="11"/>
+      <c r="F1" s="20" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -668,20 +668,20 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="19">
         <v>5</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -689,20 +689,20 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="19">
         <v>7</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -710,15 +710,15 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="F4" s="11"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -726,14 +726,14 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="22"/>
       <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="20"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F7" s="8" t="s">
@@ -749,7 +749,7 @@
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -757,13 +757,13 @@
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="17">
         <v>1</v>
       </c>
     </row>
@@ -771,7 +771,7 @@
       <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="18" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added on reaction methods
</commit_message>
<xml_diff>
--- a/Files/Parameter Optimization_Planning Sheet.xlsx
+++ b/Files/Parameter Optimization_Planning Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivikram\OneDrive\Git Hub\API\AUTOMATION\parameter_optimization\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2d90ee17b1e0b34/Git Hub/API/AUTOMATION/parameter_optimization/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D796473-49F0-42ED-A728-9DAC3B26F8FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{6D796473-49F0-42ED-A728-9DAC3B26F8FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BA7A91B4-4601-42DB-8653-54AD8C60E365}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Parameter</t>
   </si>
@@ -78,12 +78,6 @@
     <t>Max</t>
   </si>
   <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
     <t>Example 1</t>
   </si>
   <si>
@@ -108,23 +102,22 @@
     <t>Optimal Tunning Parameter</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Start from
-excel</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>Sharpe Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min </t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>Select a state to perform operation</t>
   </si>
 </sst>
 </file>
@@ -163,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,13 +195,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,15 +236,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -295,11 +285,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -307,33 +306,38 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -342,8 +346,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,174 +629,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13">
+      <c r="B1" s="8">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="F1" s="20" t="s">
+      <c r="C1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>10</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="G1" s="4" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="19">
-        <v>5</v>
-      </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="1" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="19">
-        <v>7</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="1" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="1" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="1" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F7" s="8" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="12"/>
+      <c r="E7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="13"/>
+      <c r="E8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F8" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:F5"/>
+  <mergeCells count="2">
+    <mergeCell ref="E1:E5"/>
+    <mergeCell ref="D10:E10"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11" xr:uid="{D917662C-A9DC-4E02-9AFF-5FD1F2BAC8E5}">
+      <formula1>"SELECT,READY,MODIFY"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated excel sheet format
</commit_message>
<xml_diff>
--- a/Files/Parameter Optimization_Planning Sheet.xlsx
+++ b/Files/Parameter Optimization_Planning Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2d90ee17b1e0b34/Git Hub/API/AUTOMATION/parameter_optimization/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{6D796473-49F0-42ED-A728-9DAC3B26F8FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BA7A91B4-4601-42DB-8653-54AD8C60E365}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F185C1FB-A913-4AFB-AC6D-B731C6BC97AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,24 +36,6 @@
     <t>RSI</t>
   </si>
   <si>
-    <t xml:space="preserve">Tunning Parameter 1 </t>
-  </si>
-  <si>
-    <t>Period/window size</t>
-  </si>
-  <si>
-    <t>Tunning Parameter 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entry Cutoff </t>
-  </si>
-  <si>
-    <t>Tunning Parameter 3</t>
-  </si>
-  <si>
-    <t>Exit Cutoff</t>
-  </si>
-  <si>
     <t>Experiment No</t>
   </si>
   <si>
@@ -63,21 +45,12 @@
     <t>Return%</t>
   </si>
   <si>
-    <t>Risk%</t>
-  </si>
-  <si>
-    <t>Sharp Ratio</t>
-  </si>
-  <si>
     <t>Maximum Drawdown</t>
   </si>
   <si>
     <t>Objective</t>
   </si>
   <si>
-    <t>Max</t>
-  </si>
-  <si>
     <t>Example 1</t>
   </si>
   <si>
@@ -90,41 +63,68 @@
     <t>Findout the Tunning parameter 1 which gives the maximum return.</t>
   </si>
   <si>
-    <t>Tunning Parameter 1: RSI Window size</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>Maximum Return</t>
-  </si>
-  <si>
-    <t>Optimal Tunning Parameter</t>
-  </si>
-  <si>
     <t>Sharpe Ratio</t>
   </si>
   <si>
-    <t xml:space="preserve">Min </t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
+    <t>Loss%</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunning Parameter  </t>
+  </si>
+  <si>
+    <t>Max Loss %</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>Max(Excludes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min(Includes) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunning Parameter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max </t>
+  </si>
+  <si>
+    <t>Maximum return</t>
+  </si>
+  <si>
+    <t>Minimum Loss</t>
+  </si>
+  <si>
+    <t>In between a certain range</t>
+  </si>
+  <si>
+    <t>Optimized Parameter</t>
+  </si>
+  <si>
     <t>SELECT</t>
   </si>
   <si>
-    <t>Select a state to perform operation</t>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Value(%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +141,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
@@ -148,15 +179,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,18 +225,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -239,43 +299,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -294,11 +317,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -312,49 +357,80 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC0099"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -629,198 +705,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="8">
+        <v>3</v>
+      </c>
+      <c r="B1" s="26">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>10</v>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="34"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="22"/>
+      <c r="I3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="C5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="35">
+        <v>-100.16</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="G6" s="14" t="str">
+        <f>IF(B3="Window","Entry, Exit",IF(B3="Entry","Window, Exit","Window, Entry"))</f>
+        <v>Entry, Exit</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="9" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="7"/>
+      <c r="F7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="G8" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="12"/>
-      <c r="E7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="13"/>
-      <c r="E8" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="27"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>25</v>
-      </c>
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E1:E5"/>
-    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11" xr:uid="{D917662C-A9DC-4E02-9AFF-5FD1F2BAC8E5}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{D917662C-A9DC-4E02-9AFF-5FD1F2BAC8E5}">
       <formula1>"SELECT,READY,MODIFY"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{20AA2624-69A6-4D1E-8FFB-1CCA9DC3D64E}">
+      <formula1>"Window,Entry,Exit"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>